<commit_message>
Update Code for efficiency
</commit_message>
<xml_diff>
--- a/ASINs to Forecast.xlsx
+++ b/ASINs to Forecast.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gigabyte365-my.sharepoint.com/personal/charleshsu_gigabyteusa_com/Documents/Documents/GitHub/Forecast Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{45AAEFF9-7462-448C-81ED-DE8115A57EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE909B4A-6EC0-4FF7-B1C0-6C4DB438E6D5}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{45AAEFF9-7462-448C-81ED-DE8115A57EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC962774-4217-4511-BAD7-778E2948717E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{134BD2A0-BBF2-4515-A7F2-D8D2375BE721}"/>
+    <workbookView xWindow="61890" yWindow="2730" windowWidth="7500" windowHeight="15345" xr2:uid="{134BD2A0-BBF2-4515-A7F2-D8D2375BE721}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,141 +36,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ASIN</t>
   </si>
   <si>
-    <t>B0CSTCZMQ5</t>
-  </si>
-  <si>
-    <t>B0BTJYYTGM</t>
-  </si>
-  <si>
-    <t>B0BTK4H5VS</t>
-  </si>
-  <si>
-    <t>B09VKFM255</t>
-  </si>
-  <si>
-    <t>B0BZFVFTWC</t>
-  </si>
-  <si>
-    <t>B09VK35VYJ</t>
-  </si>
-  <si>
-    <t>B09VKF3CFC</t>
-  </si>
-  <si>
-    <t>B0CKM1JX4S</t>
-  </si>
-  <si>
-    <t>B0BSMJM9D7</t>
-  </si>
-  <si>
-    <t>B09RK7GFQL</t>
-  </si>
-  <si>
-    <t>B09VK3TVK2</t>
-  </si>
-  <si>
-    <t>B09VK3W3Y3</t>
-  </si>
-  <si>
-    <t>B079SSKYWB</t>
-  </si>
-  <si>
-    <t>B08DKJJFW6</t>
-  </si>
-  <si>
-    <t>B08BT9CJYX</t>
-  </si>
-  <si>
-    <t>B08JGPBML2</t>
-  </si>
-  <si>
-    <t>B08DK7YPX4</t>
-  </si>
-  <si>
-    <t>B07ZS9GZRY</t>
-  </si>
-  <si>
-    <t>B07HCXL27D</t>
-  </si>
-  <si>
-    <t>B09T39WL99</t>
-  </si>
-  <si>
-    <t>B0CPQBJ3JW</t>
-  </si>
-  <si>
-    <t>B08YMY8ZZ3</t>
-  </si>
-  <si>
-    <t>B08YMVNQDJ</t>
-  </si>
-  <si>
-    <t>B0CPQ8V6LM</t>
-  </si>
-  <si>
-    <t>B0CPQ9M15Y</t>
-  </si>
-  <si>
-    <t>B0CPQML6TS</t>
-  </si>
-  <si>
-    <t>B0CPQ88F7X</t>
-  </si>
-  <si>
-    <t>B0CPQ8XM9Z</t>
-  </si>
-  <si>
-    <t>B09N74MYL7</t>
-  </si>
-  <si>
-    <t>B09T2QWDYY</t>
-  </si>
-  <si>
-    <t>B07W5LSX71</t>
-  </si>
-  <si>
-    <t>B09T5WL6YW</t>
-  </si>
-  <si>
-    <t>B09T5SDSYX</t>
-  </si>
-  <si>
-    <t>B08YMLHP1Z</t>
-  </si>
-  <si>
-    <t>B07YZ26VVQ</t>
-  </si>
-  <si>
-    <t>B07YZ2NCR5</t>
-  </si>
-  <si>
-    <t>B0DJMVRMM5</t>
-  </si>
-  <si>
-    <t>B0DJMWKGLN</t>
-  </si>
-  <si>
-    <t>B0DJMVYK9B</t>
-  </si>
-  <si>
-    <t>B0DJMXBKN4</t>
-  </si>
-  <si>
-    <t>B0DL78MJMY</t>
-  </si>
-  <si>
-    <t>B0DL7LNS2H</t>
-  </si>
-  <si>
-    <t>B0DL7T732W</t>
-  </si>
-  <si>
-    <t>B0DL717JPS</t>
+    <t>B0C4BH2Z7D</t>
+  </si>
+  <si>
+    <t>B0C4BKJCWV</t>
+  </si>
+  <si>
+    <t>B0CDNCNBSP</t>
+  </si>
+  <si>
+    <t>B0CDP24LW9</t>
+  </si>
+  <si>
+    <t>B091ZG1ZC6</t>
+  </si>
+  <si>
+    <t>B09SBV8M5F</t>
+  </si>
+  <si>
+    <t>B0CXZK5JGC</t>
+  </si>
+  <si>
+    <t>B08XY93JT3</t>
+  </si>
+  <si>
+    <t>B07G5RD1XK</t>
+  </si>
+  <si>
+    <t>B09MDTM5Z6</t>
+  </si>
+  <si>
+    <t>B08FCY3BM2</t>
+  </si>
+  <si>
+    <t>B0BHM59TQB</t>
+  </si>
+  <si>
+    <t>B07TJX83W2</t>
+  </si>
+  <si>
+    <t>B07QJ756H8</t>
+  </si>
+  <si>
+    <t>B083GTQPXF</t>
+  </si>
+  <si>
+    <t>B07TJWZGL9</t>
+  </si>
+  <si>
+    <t>B084KGJDDM</t>
+  </si>
+  <si>
+    <t>B099ZF7M85</t>
+  </si>
+  <si>
+    <t>B0CKHM2ZQ6</t>
+  </si>
+  <si>
+    <t>B07GBZL93X</t>
+  </si>
+  <si>
+    <t>B08FWY81LM</t>
+  </si>
+  <si>
+    <t>B07Z9YBT3T</t>
+  </si>
+  <si>
+    <t>B091ZFTQQ1</t>
+  </si>
+  <si>
+    <t>B07QBVWCQL</t>
+  </si>
+  <si>
+    <t>B07GJKR7RX</t>
+  </si>
+  <si>
+    <t>B08XY9146V</t>
+  </si>
+  <si>
+    <t>B07VV87QVL</t>
   </si>
 </sst>
 </file>
@@ -546,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239AF9F6-03F5-416E-B32F-31827F3AFA12}">
-  <dimension ref="A1:A45"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AI11" sqref="AI11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,91 +643,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>44</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>